<commit_message>
Remove xz1018-t sample from all worksheets
</commit_message>
<xml_diff>
--- a/DataRepo/example_data/obob_maven_c160_serum.xlsx
+++ b/DataRepo/example_data/obob_maven_c160_serum.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="446" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="443" uniqueCount="54">
   <si>
     <t xml:space="preserve">label</t>
   </si>
@@ -186,9 +186,6 @@
   <si>
     <t xml:space="preserve">C_Label</t>
   </si>
-  <si>
-    <t xml:space="preserve">xz1018-t</t>
-  </si>
 </sst>
 </file>
 
@@ -300,11 +297,12 @@
   <dimension ref="A1:AMJ54"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="S1" activeCellId="0" sqref="S1"/>
+      <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="12.68"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="11.52"/>
   </cols>
   <sheetData>
@@ -3190,15 +3188,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G94"/>
+  <dimension ref="A1:AMJ94"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="11.52"/>
+  </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" s="1" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>52</v>
       </c>
@@ -3217,11 +3218,9 @@
       <c r="F1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AMJ1" s="0"/>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>19</v>
       </c>
@@ -3240,11 +3239,8 @@
       <c r="F2" s="0" t="n">
         <v>1762421928.88546</v>
       </c>
-      <c r="G2" s="0" t="n">
-        <v>1033226822.36885</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>19</v>
       </c>
@@ -3263,11 +3259,8 @@
       <c r="F3" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="G3" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
         <v>19</v>
       </c>
@@ -3286,11 +3279,8 @@
       <c r="F4" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="G4" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
         <v>19</v>
       </c>
@@ -3309,11 +3299,8 @@
       <c r="F5" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="G5" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
         <v>19</v>
       </c>
@@ -3332,11 +3319,8 @@
       <c r="F6" s="0" t="n">
         <v>204364.89094726</v>
       </c>
-      <c r="G6" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
         <v>19</v>
       </c>
@@ -3355,11 +3339,8 @@
       <c r="F7" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="G7" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
         <v>19</v>
       </c>
@@ -3378,11 +3359,8 @@
       <c r="F8" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="G8" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
         <v>19</v>
       </c>
@@ -3401,11 +3379,8 @@
       <c r="F9" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="G9" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
         <v>19</v>
       </c>
@@ -3424,11 +3399,8 @@
       <c r="F10" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="G10" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
         <v>19</v>
       </c>
@@ -3447,11 +3419,8 @@
       <c r="F11" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="G11" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
         <v>19</v>
       </c>
@@ -3470,11 +3439,8 @@
       <c r="F12" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="G12" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
         <v>19</v>
       </c>
@@ -3493,11 +3459,8 @@
       <c r="F13" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="G13" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
         <v>19</v>
       </c>
@@ -3516,11 +3479,8 @@
       <c r="F14" s="0" t="n">
         <v>289542.161667861</v>
       </c>
-      <c r="G14" s="0" t="n">
-        <v>63453.6653472893</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
         <v>19</v>
       </c>
@@ -3539,11 +3499,8 @@
       <c r="F15" s="0" t="n">
         <v>569033.077733821</v>
       </c>
-      <c r="G15" s="0" t="n">
-        <v>104770.750853828</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
         <v>19</v>
       </c>
@@ -3562,11 +3519,8 @@
       <c r="F16" s="0" t="n">
         <v>2062655.82133341</v>
       </c>
-      <c r="G16" s="0" t="n">
-        <v>946089.032433367</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
         <v>19</v>
       </c>
@@ -3585,11 +3539,8 @@
       <c r="F17" s="0" t="n">
         <v>9069961.78322296</v>
       </c>
-      <c r="G17" s="0" t="n">
-        <v>3029552.24397228</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
         <v>19</v>
       </c>
@@ -3608,11 +3559,8 @@
       <c r="F18" s="0" t="n">
         <v>280988425.008348</v>
       </c>
-      <c r="G18" s="0" t="n">
-        <v>139868960.005772</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
         <v>32</v>
       </c>
@@ -3631,11 +3579,8 @@
       <c r="F19" s="0" t="n">
         <v>2405744350.0857</v>
       </c>
-      <c r="G19" s="0" t="n">
-        <v>1711939100.17907</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
         <v>32</v>
       </c>
@@ -3654,11 +3599,8 @@
       <c r="F20" s="0" t="n">
         <v>3017375.69948149</v>
       </c>
-      <c r="G20" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
         <v>32</v>
       </c>
@@ -3677,11 +3619,8 @@
       <c r="F21" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="G21" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
         <v>32</v>
       </c>
@@ -3700,11 +3639,8 @@
       <c r="F22" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="G22" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
         <v>32</v>
       </c>
@@ -3723,11 +3659,8 @@
       <c r="F23" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="G23" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
         <v>32</v>
       </c>
@@ -3746,11 +3679,8 @@
       <c r="F24" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="G24" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
         <v>32</v>
       </c>
@@ -3769,11 +3699,8 @@
       <c r="F25" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="G25" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
         <v>32</v>
       </c>
@@ -3792,11 +3719,8 @@
       <c r="F26" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="G26" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
         <v>32</v>
       </c>
@@ -3815,11 +3739,8 @@
       <c r="F27" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="G27" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
         <v>32</v>
       </c>
@@ -3838,11 +3759,8 @@
       <c r="F28" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="G28" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
         <v>32</v>
       </c>
@@ -3861,11 +3779,8 @@
       <c r="F29" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="G29" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
         <v>32</v>
       </c>
@@ -3884,11 +3799,8 @@
       <c r="F30" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="G30" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
         <v>32</v>
       </c>
@@ -3907,11 +3819,8 @@
       <c r="F31" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="G31" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
         <v>32</v>
       </c>
@@ -3930,11 +3839,8 @@
       <c r="F32" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="G32" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
         <v>32</v>
       </c>
@@ -3953,11 +3859,8 @@
       <c r="F33" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="G33" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
         <v>32</v>
       </c>
@@ -3976,11 +3879,8 @@
       <c r="F34" s="0" t="n">
         <v>19641.6131037296</v>
       </c>
-      <c r="G34" s="0" t="n">
-        <v>153683.16695405</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
         <v>32</v>
       </c>
@@ -3999,11 +3899,8 @@
       <c r="F35" s="0" t="n">
         <v>2063240.33531935</v>
       </c>
-      <c r="G35" s="0" t="n">
-        <v>1479738.99079315</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
         <v>32</v>
       </c>
@@ -4022,11 +3919,8 @@
       <c r="F36" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="G36" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
         <v>32</v>
       </c>
@@ -4045,11 +3939,8 @@
       <c r="F37" s="0" t="n">
         <v>389053.942958031</v>
       </c>
-      <c r="G37" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
         <v>35</v>
       </c>
@@ -4068,11 +3959,8 @@
       <c r="F38" s="0" t="n">
         <v>1326394925.40081</v>
       </c>
-      <c r="G38" s="0" t="n">
-        <v>964530499.528873</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
         <v>35</v>
       </c>
@@ -4091,11 +3979,8 @@
       <c r="F39" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="G39" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
         <v>35</v>
       </c>
@@ -4114,11 +3999,8 @@
       <c r="F40" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="G40" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
         <v>35</v>
       </c>
@@ -4137,11 +4019,8 @@
       <c r="F41" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="G41" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
         <v>35</v>
       </c>
@@ -4160,11 +4039,8 @@
       <c r="F42" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="G42" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
         <v>35</v>
       </c>
@@ -4183,11 +4059,8 @@
       <c r="F43" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="G43" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
         <v>35</v>
       </c>
@@ -4206,11 +4079,8 @@
       <c r="F44" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="G44" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
         <v>35</v>
       </c>
@@ -4229,11 +4099,8 @@
       <c r="F45" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="G45" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
         <v>35</v>
       </c>
@@ -4252,11 +4119,8 @@
       <c r="F46" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="G46" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
         <v>35</v>
       </c>
@@ -4275,11 +4139,8 @@
       <c r="F47" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="G47" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
         <v>35</v>
       </c>
@@ -4298,11 +4159,8 @@
       <c r="F48" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="G48" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
         <v>35</v>
       </c>
@@ -4321,11 +4179,8 @@
       <c r="F49" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="G49" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
         <v>35</v>
       </c>
@@ -4344,11 +4199,8 @@
       <c r="F50" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="G50" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
         <v>35</v>
       </c>
@@ -4367,11 +4219,8 @@
       <c r="F51" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="G51" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
         <v>35</v>
       </c>
@@ -4390,11 +4239,8 @@
       <c r="F52" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="G52" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
         <v>35</v>
       </c>
@@ -4413,11 +4259,8 @@
       <c r="F53" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="G53" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
         <v>35</v>
       </c>
@@ -4436,11 +4279,8 @@
       <c r="F54" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="G54" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
         <v>35</v>
       </c>
@@ -4459,11 +4299,8 @@
       <c r="F55" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="G55" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
         <v>35</v>
       </c>
@@ -4482,11 +4319,8 @@
       <c r="F56" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="G56" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
         <v>37</v>
       </c>
@@ -4505,11 +4339,8 @@
       <c r="F57" s="0" t="n">
         <v>23210750.5617758</v>
       </c>
-      <c r="G57" s="0" t="n">
-        <v>33677918.8655511</v>
-      </c>
-    </row>
-    <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
         <v>37</v>
       </c>
@@ -4528,11 +4359,8 @@
       <c r="F58" s="0" t="n">
         <v>478088.471263683</v>
       </c>
-      <c r="G58" s="0" t="n">
-        <v>506758.674645109</v>
-      </c>
-    </row>
-    <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
         <v>37</v>
       </c>
@@ -4551,11 +4379,8 @@
       <c r="F59" s="0" t="n">
         <v>54781.1969973452</v>
       </c>
-      <c r="G59" s="0" t="n">
-        <v>62903.8274007506</v>
-      </c>
-    </row>
-    <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
         <v>37</v>
       </c>
@@ -4574,11 +4399,8 @@
       <c r="F60" s="0" t="n">
         <v>7658.10768844218</v>
       </c>
-      <c r="G60" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
         <v>37</v>
       </c>
@@ -4597,11 +4419,8 @@
       <c r="F61" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="G61" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
         <v>37</v>
       </c>
@@ -4620,11 +4439,8 @@
       <c r="F62" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="G62" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
         <v>37</v>
       </c>
@@ -4643,11 +4459,8 @@
       <c r="F63" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="G63" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
         <v>40</v>
       </c>
@@ -4666,11 +4479,8 @@
       <c r="F64" s="0" t="n">
         <v>48724332.6935433</v>
       </c>
-      <c r="G64" s="0" t="n">
-        <v>105370988.019046</v>
-      </c>
-    </row>
-    <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
         <v>40</v>
       </c>
@@ -4689,11 +4499,8 @@
       <c r="F65" s="0" t="n">
         <v>529678.354151628</v>
       </c>
-      <c r="G65" s="0" t="n">
-        <v>756494.227354507</v>
-      </c>
-    </row>
-    <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
         <v>40</v>
       </c>
@@ -4712,11 +4519,8 @@
       <c r="F66" s="0" t="n">
         <v>62500.2532296836</v>
       </c>
-      <c r="G66" s="0" t="n">
-        <v>107293.503038414</v>
-      </c>
-    </row>
-    <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
         <v>40</v>
       </c>
@@ -4735,11 +4539,8 @@
       <c r="F67" s="0" t="n">
         <v>17391.4194960218</v>
       </c>
-      <c r="G67" s="0" t="n">
-        <v>22742.0265153947</v>
-      </c>
-    </row>
-    <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
         <v>42</v>
       </c>
@@ -4758,11 +4559,8 @@
       <c r="F68" s="0" t="n">
         <v>75747183.6464512</v>
       </c>
-      <c r="G68" s="0" t="n">
-        <v>24772780.1023765</v>
-      </c>
-    </row>
-    <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
         <v>42</v>
       </c>
@@ -4781,11 +4579,8 @@
       <c r="F69" s="0" t="n">
         <v>89939.6583739246</v>
       </c>
-      <c r="G69" s="0" t="n">
-        <v>1180.46891393405</v>
-      </c>
-    </row>
-    <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
         <v>42</v>
       </c>
@@ -4804,11 +4599,8 @@
       <c r="F70" s="0" t="n">
         <v>4138299.39931089</v>
       </c>
-      <c r="G70" s="0" t="n">
-        <v>717728.048814273</v>
-      </c>
-    </row>
-    <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
         <v>42</v>
       </c>
@@ -4827,11 +4619,8 @@
       <c r="F71" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="G71" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
         <v>42</v>
       </c>
@@ -4850,11 +4639,8 @@
       <c r="F72" s="0" t="n">
         <v>55727.0962698365</v>
       </c>
-      <c r="G72" s="0" t="n">
-        <v>8985.03944013996</v>
-      </c>
-    </row>
-    <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
         <v>44</v>
       </c>
@@ -4873,11 +4659,8 @@
       <c r="F73" s="0" t="n">
         <v>21623870.034669</v>
       </c>
-      <c r="G73" s="0" t="n">
-        <v>16363545.6343464</v>
-      </c>
-    </row>
-    <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
         <v>44</v>
       </c>
@@ -4896,11 +4679,8 @@
       <c r="F74" s="0" t="n">
         <v>170067.827366881</v>
       </c>
-      <c r="G74" s="0" t="n">
-        <v>234804.127237947</v>
-      </c>
-    </row>
-    <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
         <v>44</v>
       </c>
@@ -4919,11 +4699,8 @@
       <c r="F75" s="0" t="n">
         <v>349029.424105241</v>
       </c>
-      <c r="G75" s="0" t="n">
-        <v>170729.820791629</v>
-      </c>
-    </row>
-    <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
         <v>44</v>
       </c>
@@ -4942,11 +4719,8 @@
       <c r="F76" s="0" t="n">
         <v>8323.39289093685</v>
       </c>
-      <c r="G76" s="0" t="n">
-        <v>990.696351533298</v>
-      </c>
-    </row>
-    <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
         <v>44</v>
       </c>
@@ -4965,11 +4739,8 @@
       <c r="F77" s="0" t="n">
         <v>941.655549057584</v>
       </c>
-      <c r="G77" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
         <v>44</v>
       </c>
@@ -4988,11 +4759,8 @@
       <c r="F78" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="G78" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
         <v>46</v>
       </c>
@@ -5011,11 +4779,8 @@
       <c r="F79" s="0" t="n">
         <v>1263449.19091546</v>
       </c>
-      <c r="G79" s="0" t="n">
-        <v>2711801.33230197</v>
-      </c>
-    </row>
-    <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
         <v>46</v>
       </c>
@@ -5034,11 +4799,8 @@
       <c r="F80" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="G80" s="0" t="n">
-        <v>9458.48436336872</v>
-      </c>
-    </row>
-    <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="s">
         <v>46</v>
       </c>
@@ -5057,11 +4819,8 @@
       <c r="F81" s="0" t="n">
         <v>1610.95415534557</v>
       </c>
-      <c r="G81" s="0" t="n">
-        <v>833.230592171133</v>
-      </c>
-    </row>
-    <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
         <v>46</v>
       </c>
@@ -5080,11 +4839,8 @@
       <c r="F82" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="G82" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
         <v>48</v>
       </c>
@@ -5103,11 +4859,8 @@
       <c r="F83" s="0" t="n">
         <v>145963.62897335</v>
       </c>
-      <c r="G83" s="0" t="n">
-        <v>1164986.90170033</v>
-      </c>
-    </row>
-    <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="s">
         <v>48</v>
       </c>
@@ -5126,11 +4879,8 @@
       <c r="F84" s="0" t="n">
         <v>2006.17814286056</v>
       </c>
-      <c r="G84" s="0" t="n">
-        <v>18422.7279083831</v>
-      </c>
-    </row>
-    <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="s">
         <v>48</v>
       </c>
@@ -5149,11 +4899,8 @@
       <c r="F85" s="0" t="n">
         <v>2202.89630862544</v>
       </c>
-      <c r="G85" s="0" t="n">
-        <v>16758.9584776041</v>
-      </c>
-    </row>
-    <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="s">
         <v>48</v>
       </c>
@@ -5172,11 +4919,8 @@
       <c r="F86" s="0" t="n">
         <v>544.327484504929</v>
       </c>
-      <c r="G86" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="s">
         <v>48</v>
       </c>
@@ -5195,11 +4939,8 @@
       <c r="F87" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="G87" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="s">
         <v>48</v>
       </c>
@@ -5218,11 +4959,8 @@
       <c r="F88" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="G88" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="s">
         <v>48</v>
       </c>
@@ -5241,11 +4979,8 @@
       <c r="F89" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="G89" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="s">
         <v>50</v>
       </c>
@@ -5264,11 +4999,8 @@
       <c r="F90" s="0" t="n">
         <v>970003.347150831</v>
       </c>
-      <c r="G90" s="0" t="n">
-        <v>7269196.64586176</v>
-      </c>
-    </row>
-    <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="s">
         <v>50</v>
       </c>
@@ -5287,11 +5019,8 @@
       <c r="F91" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="G91" s="0" t="n">
-        <v>74554.2613405521</v>
-      </c>
-    </row>
-    <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="s">
         <v>50</v>
       </c>
@@ -5310,11 +5039,8 @@
       <c r="F92" s="0" t="n">
         <v>8351.90947294179</v>
       </c>
-      <c r="G92" s="0" t="n">
-        <v>76312.1255627973</v>
-      </c>
-    </row>
-    <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="s">
         <v>50</v>
       </c>
@@ -5333,11 +5059,8 @@
       <c r="F93" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="G93" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="0" t="s">
         <v>50</v>
       </c>
@@ -5354,9 +5077,6 @@
         <v>0</v>
       </c>
       <c r="F94" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G94" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -5376,15 +5096,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G94"/>
+  <dimension ref="A1:AMJ94"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="11.52"/>
+  </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" s="1" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>52</v>
       </c>
@@ -5403,11 +5126,9 @@
       <c r="F1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AMJ1" s="0"/>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>19</v>
       </c>
@@ -5426,11 +5147,8 @@
       <c r="F2" s="0" t="n">
         <v>0.857373448342073</v>
       </c>
-      <c r="G2" s="0" t="n">
-        <v>0.877669065992794</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>19</v>
       </c>
@@ -5449,11 +5167,8 @@
       <c r="F3" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="G3" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
         <v>19</v>
       </c>
@@ -5472,11 +5187,8 @@
       <c r="F4" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="G4" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
         <v>19</v>
       </c>
@@ -5495,11 +5207,8 @@
       <c r="F5" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="G5" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
         <v>19</v>
       </c>
@@ -5518,11 +5227,8 @@
       <c r="F6" s="0" t="n">
         <v>9.94183222528953E-005</v>
       </c>
-      <c r="G6" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
         <v>19</v>
       </c>
@@ -5541,11 +5247,8 @@
       <c r="F7" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="G7" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
         <v>19</v>
       </c>
@@ -5564,11 +5267,8 @@
       <c r="F8" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="G8" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
         <v>19</v>
       </c>
@@ -5587,11 +5287,8 @@
       <c r="F9" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="G9" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
         <v>19</v>
       </c>
@@ -5610,11 +5307,8 @@
       <c r="F10" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="G10" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
         <v>19</v>
       </c>
@@ -5633,11 +5327,8 @@
       <c r="F11" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="G11" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
         <v>19</v>
       </c>
@@ -5656,11 +5347,8 @@
       <c r="F12" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="G12" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
         <v>19</v>
       </c>
@@ -5679,11 +5367,8 @@
       <c r="F13" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="G13" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
         <v>19</v>
       </c>
@@ -5702,11 +5387,8 @@
       <c r="F14" s="0" t="n">
         <v>0.000140854898319712</v>
       </c>
-      <c r="G14" s="0" t="n">
-        <v>5.39003808200534E-005</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
         <v>19</v>
       </c>
@@ -5725,11 +5407,8 @@
       <c r="F15" s="0" t="n">
         <v>0.000276820121266804</v>
       </c>
-      <c r="G15" s="0" t="n">
-        <v>8.89969608361719E-005</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
         <v>19</v>
       </c>
@@ -5748,11 +5427,8 @@
       <c r="F16" s="0" t="n">
         <v>0.00100342960178545</v>
       </c>
-      <c r="G16" s="0" t="n">
-        <v>0.000803650330658366</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
         <v>19</v>
       </c>
@@ -5771,11 +5447,8 @@
       <c r="F17" s="0" t="n">
         <v>0.00441230574981007</v>
       </c>
-      <c r="G17" s="0" t="n">
-        <v>0.00257343714930613</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
         <v>19</v>
       </c>
@@ -5794,11 +5467,8 @@
       <c r="F18" s="0" t="n">
         <v>0.136693722964492</v>
       </c>
-      <c r="G18" s="0" t="n">
-        <v>0.118810949185585</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
         <v>32</v>
       </c>
@@ -5817,11 +5487,8 @@
       <c r="F19" s="0" t="n">
         <v>0.997723442701507</v>
       </c>
-      <c r="G19" s="0" t="n">
-        <v>0.9990467738386</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
         <v>32</v>
       </c>
@@ -5840,11 +5507,8 @@
       <c r="F20" s="0" t="n">
         <v>0.00125138253809192</v>
       </c>
-      <c r="G20" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
         <v>32</v>
       </c>
@@ -5863,11 +5527,8 @@
       <c r="F21" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="G21" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
         <v>32</v>
       </c>
@@ -5886,11 +5547,8 @@
       <c r="F22" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="G22" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
         <v>32</v>
       </c>
@@ -5909,11 +5567,8 @@
       <c r="F23" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="G23" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
         <v>32</v>
       </c>
@@ -5932,11 +5587,8 @@
       <c r="F24" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="G24" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
         <v>32</v>
       </c>
@@ -5955,11 +5607,8 @@
       <c r="F25" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="G25" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
         <v>32</v>
       </c>
@@ -5978,11 +5627,8 @@
       <c r="F26" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="G26" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
         <v>32</v>
       </c>
@@ -6001,11 +5647,8 @@
       <c r="F27" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="G27" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
         <v>32</v>
       </c>
@@ -6024,11 +5667,8 @@
       <c r="F28" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="G28" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
         <v>32</v>
       </c>
@@ -6047,11 +5687,8 @@
       <c r="F29" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="G29" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
         <v>32</v>
       </c>
@@ -6070,11 +5707,8 @@
       <c r="F30" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="G30" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
         <v>32</v>
       </c>
@@ -6093,11 +5727,8 @@
       <c r="F31" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="G31" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
         <v>32</v>
       </c>
@@ -6116,11 +5747,8 @@
       <c r="F32" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="G32" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
         <v>32</v>
       </c>
@@ -6139,11 +5767,8 @@
       <c r="F33" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="G33" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
         <v>32</v>
       </c>
@@ -6162,11 +5787,8 @@
       <c r="F34" s="0" t="n">
         <v>8.14587711506668E-006</v>
       </c>
-      <c r="G34" s="0" t="n">
-        <v>8.96858259284356E-005</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
         <v>32</v>
       </c>
@@ -6185,11 +5807,8 @@
       <c r="F35" s="0" t="n">
         <v>0.000855678306135106</v>
       </c>
-      <c r="G35" s="0" t="n">
-        <v>0.000863540335471305</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
         <v>32</v>
       </c>
@@ -6208,11 +5827,8 @@
       <c r="F36" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="G36" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
         <v>32</v>
       </c>
@@ -6231,11 +5847,8 @@
       <c r="F37" s="0" t="n">
         <v>0.000161350577151248</v>
       </c>
-      <c r="G37" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
         <v>35</v>
       </c>
@@ -6254,11 +5867,8 @@
       <c r="F38" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="G38" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
         <v>35</v>
       </c>
@@ -6277,11 +5887,8 @@
       <c r="F39" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="G39" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
         <v>35</v>
       </c>
@@ -6300,11 +5907,8 @@
       <c r="F40" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="G40" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
         <v>35</v>
       </c>
@@ -6323,11 +5927,8 @@
       <c r="F41" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="G41" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
         <v>35</v>
       </c>
@@ -6346,11 +5947,8 @@
       <c r="F42" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="G42" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
         <v>35</v>
       </c>
@@ -6369,11 +5967,8 @@
       <c r="F43" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="G43" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
         <v>35</v>
       </c>
@@ -6392,11 +5987,8 @@
       <c r="F44" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="G44" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
         <v>35</v>
       </c>
@@ -6415,11 +6007,8 @@
       <c r="F45" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="G45" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
         <v>35</v>
       </c>
@@ -6438,11 +6027,8 @@
       <c r="F46" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="G46" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
         <v>35</v>
       </c>
@@ -6461,11 +6047,8 @@
       <c r="F47" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="G47" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
         <v>35</v>
       </c>
@@ -6484,11 +6067,8 @@
       <c r="F48" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="G48" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
         <v>35</v>
       </c>
@@ -6507,11 +6087,8 @@
       <c r="F49" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="G49" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
         <v>35</v>
       </c>
@@ -6530,11 +6107,8 @@
       <c r="F50" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="G50" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
         <v>35</v>
       </c>
@@ -6553,11 +6127,8 @@
       <c r="F51" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="G51" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
         <v>35</v>
       </c>
@@ -6576,11 +6147,8 @@
       <c r="F52" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="G52" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
         <v>35</v>
       </c>
@@ -6599,11 +6167,8 @@
       <c r="F53" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="G53" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
         <v>35</v>
       </c>
@@ -6622,11 +6187,8 @@
       <c r="F54" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="G54" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
         <v>35</v>
       </c>
@@ -6645,11 +6207,8 @@
       <c r="F55" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="G55" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
         <v>35</v>
       </c>
@@ -6668,11 +6227,8 @@
       <c r="F56" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="G56" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
         <v>37</v>
       </c>
@@ -6691,11 +6247,8 @@
       <c r="F57" s="0" t="n">
         <v>0.977242160684424</v>
       </c>
-      <c r="G57" s="0" t="n">
-        <v>0.983366343569452</v>
-      </c>
-    </row>
-    <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
         <v>37</v>
       </c>
@@ -6714,11 +6267,8 @@
       <c r="F58" s="0" t="n">
         <v>0.0201289574592839</v>
       </c>
-      <c r="G58" s="0" t="n">
-        <v>0.0147969186263347</v>
-      </c>
-    </row>
-    <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
         <v>37</v>
       </c>
@@ -6737,11 +6287,8 @@
       <c r="F59" s="0" t="n">
         <v>0.00230645257145312</v>
       </c>
-      <c r="G59" s="0" t="n">
-        <v>0.00183673780421372</v>
-      </c>
-    </row>
-    <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
         <v>37</v>
       </c>
@@ -6760,11 +6307,8 @@
       <c r="F60" s="0" t="n">
         <v>0.00032242928483889</v>
       </c>
-      <c r="G60" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
         <v>37</v>
       </c>
@@ -6783,11 +6327,8 @@
       <c r="F61" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="G61" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
         <v>37</v>
       </c>
@@ -6806,11 +6347,8 @@
       <c r="F62" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="G62" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
         <v>37</v>
       </c>
@@ -6829,11 +6367,8 @@
       <c r="F63" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="G63" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
         <v>40</v>
       </c>
@@ -6852,11 +6387,8 @@
       <c r="F64" s="0" t="n">
         <v>0.987643993414999</v>
       </c>
-      <c r="G64" s="0" t="n">
-        <v>0.991656780852179</v>
-      </c>
-    </row>
-    <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
         <v>40</v>
       </c>
@@ -6875,11 +6407,8 @@
       <c r="F65" s="0" t="n">
         <v>0.0107365994771052</v>
       </c>
-      <c r="G65" s="0" t="n">
-        <v>0.00711944192927209</v>
-      </c>
-    </row>
-    <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
         <v>40</v>
       </c>
@@ -6898,11 +6427,8 @@
       <c r="F66" s="0" t="n">
         <v>0.00126688240303788</v>
       </c>
-      <c r="G66" s="0" t="n">
-        <v>0.00100974975967953</v>
-      </c>
-    </row>
-    <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
         <v>40</v>
       </c>
@@ -6921,11 +6447,8 @@
       <c r="F67" s="0" t="n">
         <v>0.000352524704858247</v>
       </c>
-      <c r="G67" s="0" t="n">
-        <v>0.000214027458869748</v>
-      </c>
-    </row>
-    <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
         <v>42</v>
       </c>
@@ -6944,11 +6467,8 @@
       <c r="F68" s="0" t="n">
         <v>0.946471265692937</v>
       </c>
-      <c r="G68" s="0" t="n">
-        <v>0.971455908699263</v>
-      </c>
-    </row>
-    <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
         <v>42</v>
       </c>
@@ -6967,11 +6487,8 @@
       <c r="F69" s="0" t="n">
         <v>0.0011238081496796</v>
       </c>
-      <c r="G69" s="0" t="n">
-        <v>4.62916756511726E-005</v>
-      </c>
-    </row>
-    <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
         <v>42</v>
       </c>
@@ -6990,11 +6507,8 @@
       <c r="F70" s="0" t="n">
         <v>0.0517086085809291</v>
       </c>
-      <c r="G70" s="0" t="n">
-        <v>0.0281454544454997</v>
-      </c>
-    </row>
-    <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
         <v>42</v>
       </c>
@@ -7013,11 +6527,8 @@
       <c r="F71" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="G71" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
         <v>42</v>
       </c>
@@ -7036,11 +6547,8 @@
       <c r="F72" s="0" t="n">
         <v>0.000696317576453886</v>
       </c>
-      <c r="G72" s="0" t="n">
-        <v>0.000352345179586143</v>
-      </c>
-    </row>
-    <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
         <v>44</v>
       </c>
@@ -7059,11 +6567,8 @@
       <c r="F73" s="0" t="n">
         <v>0.976148575370108</v>
       </c>
-      <c r="G73" s="0" t="n">
-        <v>0.975758918261853</v>
-      </c>
-    </row>
-    <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
         <v>44</v>
       </c>
@@ -7082,11 +6587,8 @@
       <c r="F74" s="0" t="n">
         <v>0.0076772320187972</v>
       </c>
-      <c r="G74" s="0" t="n">
-        <v>0.0140013800380903</v>
-      </c>
-    </row>
-    <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
         <v>44</v>
       </c>
@@ -7105,11 +6607,8 @@
       <c r="F75" s="0" t="n">
         <v>0.0157559481515722</v>
       </c>
-      <c r="G75" s="0" t="n">
-        <v>0.0101806264347142</v>
-      </c>
-    </row>
-    <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
         <v>44</v>
       </c>
@@ -7128,11 +6627,8 @@
       <c r="F76" s="0" t="n">
         <v>0.000375736077756077</v>
       </c>
-      <c r="G76" s="0" t="n">
-        <v>5.90752653428039E-005</v>
-      </c>
-    </row>
-    <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
         <v>44</v>
       </c>
@@ -7151,11 +6647,8 @@
       <c r="F77" s="0" t="n">
         <v>4.2508381766455E-005</v>
       </c>
-      <c r="G77" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
         <v>44</v>
       </c>
@@ -7174,11 +6667,8 @@
       <c r="F78" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="G78" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
         <v>46</v>
       </c>
@@ -7197,11 +6687,8 @@
       <c r="F79" s="0" t="n">
         <v>0.998726578999724</v>
       </c>
-      <c r="G79" s="0" t="n">
-        <v>0.99621919060926</v>
-      </c>
-    </row>
-    <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
         <v>46</v>
       </c>
@@ -7220,11 +6707,8 @@
       <c r="F80" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="G80" s="0" t="n">
-        <v>0.00347471015838275</v>
-      </c>
-    </row>
-    <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="s">
         <v>46</v>
       </c>
@@ -7243,11 +6727,8 @@
       <c r="F81" s="0" t="n">
         <v>0.00127342100027616</v>
       </c>
-      <c r="G81" s="0" t="n">
-        <v>0.000306099232357471</v>
-      </c>
-    </row>
-    <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
         <v>46</v>
       </c>
@@ -7266,11 +6747,8 @@
       <c r="F82" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="G82" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
         <v>48</v>
       </c>
@@ -7289,11 +6767,8 @@
       <c r="F83" s="0" t="n">
         <v>0.968461414696723</v>
       </c>
-      <c r="G83" s="0" t="n">
-        <v>0.970686046331137</v>
-      </c>
-    </row>
-    <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="s">
         <v>48</v>
       </c>
@@ -7312,11 +6787,8 @@
       <c r="F84" s="0" t="n">
         <v>0.0133108921450776</v>
       </c>
-      <c r="G84" s="0" t="n">
-        <v>0.015350116717984</v>
-      </c>
-    </row>
-    <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="s">
         <v>48</v>
       </c>
@@ -7335,11 +6807,8 @@
       <c r="F85" s="0" t="n">
         <v>0.0146161073857043</v>
       </c>
-      <c r="G85" s="0" t="n">
-        <v>0.0139638369508791</v>
-      </c>
-    </row>
-    <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="s">
         <v>48</v>
       </c>
@@ -7358,11 +6827,8 @@
       <c r="F86" s="0" t="n">
         <v>0.00361158577249542</v>
       </c>
-      <c r="G86" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="s">
         <v>48</v>
       </c>
@@ -7381,11 +6847,8 @@
       <c r="F87" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="G87" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="s">
         <v>48</v>
       </c>
@@ -7404,11 +6867,8 @@
       <c r="F88" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="G88" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="s">
         <v>48</v>
       </c>
@@ -7427,11 +6887,8 @@
       <c r="F89" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="G89" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="s">
         <v>50</v>
       </c>
@@ -7450,11 +6907,8 @@
       <c r="F90" s="0" t="n">
         <v>0.991463316196855</v>
       </c>
-      <c r="G90" s="0" t="n">
-        <v>0.979667775565091</v>
-      </c>
-    </row>
-    <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="s">
         <v>50</v>
       </c>
@@ -7473,11 +6927,8 @@
       <c r="F91" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="G91" s="0" t="n">
-        <v>0.0100476587612989</v>
-      </c>
-    </row>
-    <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="s">
         <v>50</v>
       </c>
@@ -7496,11 +6947,8 @@
       <c r="F92" s="0" t="n">
         <v>0.00853668380314486</v>
       </c>
-      <c r="G92" s="0" t="n">
-        <v>0.0102845656736098</v>
-      </c>
-    </row>
-    <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="s">
         <v>50</v>
       </c>
@@ -7519,11 +6967,8 @@
       <c r="F93" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="G93" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="0" t="s">
         <v>50</v>
       </c>
@@ -7540,9 +6985,6 @@
         <v>0</v>
       </c>
       <c r="F94" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G94" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -7562,15 +7004,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:AMJ11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="11.52"/>
+  </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" s="1" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>52</v>
       </c>
@@ -7586,11 +7031,9 @@
       <c r="E1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AMJ1" s="0"/>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>19</v>
       </c>
@@ -7606,11 +7049,8 @@
       <c r="E2" s="0" t="n">
         <v>2055605911.62872</v>
       </c>
-      <c r="F2" s="0" t="n">
-        <v>1177239648.06723</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>32</v>
       </c>
@@ -7626,11 +7066,8 @@
       <c r="E3" s="0" t="n">
         <v>2411233661.67657</v>
       </c>
-      <c r="F3" s="0" t="n">
-        <v>1713572522.33682</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
         <v>35</v>
       </c>
@@ -7646,11 +7083,8 @@
       <c r="E4" s="0" t="n">
         <v>1326394925.40081</v>
       </c>
-      <c r="F4" s="0" t="n">
-        <v>964530499.528873</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
         <v>37</v>
       </c>
@@ -7666,11 +7100,8 @@
       <c r="E5" s="0" t="n">
         <v>23751278.3377253</v>
       </c>
-      <c r="F5" s="0" t="n">
-        <v>34247581.3675969</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
         <v>40</v>
       </c>
@@ -7686,11 +7117,8 @@
       <c r="E6" s="0" t="n">
         <v>49333902.7204207</v>
       </c>
-      <c r="F6" s="0" t="n">
-        <v>106257517.775955</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
         <v>42</v>
       </c>
@@ -7706,11 +7134,8 @@
       <c r="E7" s="0" t="n">
         <v>80031149.8004058</v>
       </c>
-      <c r="F7" s="0" t="n">
-        <v>25500673.6595448</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
         <v>44</v>
       </c>
@@ -7726,11 +7151,8 @@
       <c r="E8" s="0" t="n">
         <v>22152232.3345811</v>
       </c>
-      <c r="F8" s="0" t="n">
-        <v>16770070.2787275</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
         <v>46</v>
       </c>
@@ -7746,11 +7168,8 @@
       <c r="E9" s="0" t="n">
         <v>1265060.14507081</v>
       </c>
-      <c r="F9" s="0" t="n">
-        <v>2722093.04725751</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
         <v>48</v>
       </c>
@@ -7766,11 +7185,8 @@
       <c r="E10" s="0" t="n">
         <v>150717.030909341</v>
       </c>
-      <c r="F10" s="0" t="n">
-        <v>1200168.58808632</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
         <v>50</v>
       </c>
@@ -7785,9 +7201,6 @@
       </c>
       <c r="E11" s="0" t="n">
         <v>978355.256623773</v>
-      </c>
-      <c r="F11" s="0" t="n">
-        <v>7420063.03276511</v>
       </c>
     </row>
   </sheetData>

</xml_diff>